<commit_message>
test for empty mail
</commit_message>
<xml_diff>
--- a/tests/data/test_database.xlsx
+++ b/tests/data/test_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lukas/Documents/Programming/Git/STVadmin_processing/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E89F34E-3B9C-1547-A17A-CBE43EAF15DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EEBE2A-E584-3C49-8617-AF51FA1F3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mitglieder" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>MITGLIEDERNR</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>Kitu</t>
+  </si>
+  <si>
+    <t>vorname4</t>
+  </si>
+  <si>
+    <t>nachname4</t>
+  </si>
+  <si>
+    <t>strasse4</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
@@ -494,7 +506,7 @@
   <dimension ref="A1:L651"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -647,14 +659,30 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3">
+        <v>20183</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -9717,6 +9745,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100323BBB44CBC34B469A1DE5293C6D0B60" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="276948e60e12b80fbcc8175325eeec0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ffeec27-f743-4238-9a75-26d06b1dc244" xmlns:ns3="b1372d0e-cfd1-448a-8334-bdb60fa40727" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f8a3288ef1069d34167e98cc5762b0e" ns2:_="" ns3:_="">
     <xsd:import namespace="1ffeec27-f743-4238-9a75-26d06b1dc244"/>
@@ -9951,15 +9988,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9972,6 +10000,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2696125F-A2E3-4A84-905B-AE58970A1170}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F58B1DC-7389-44C7-B847-A27685736F04}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9990,14 +10026,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2696125F-A2E3-4A84-905B-AE58970A1170}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6CEBCB2-FF40-4D9B-BFCF-7AA5436CE48A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
working for regular use
</commit_message>
<xml_diff>
--- a/tests/data/test_database.xlsx
+++ b/tests/data/test_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lukas/Documents/Programming/Git/STVadmin_processing/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EEBE2A-E584-3C49-8617-AF51FA1F3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CC87F7-8CE4-E544-86D9-88EB0FB71D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,9 +127,6 @@
     <t>Aktive Turner</t>
   </si>
   <si>
-    <t>Kitu</t>
-  </si>
-  <si>
     <t>vorname4</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>Kitu (Kinder)</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:L651"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +613,7 @@
         <v>36558</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>29</v>
@@ -663,16 +663,16 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
@@ -9745,12 +9745,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1ffeec27-f743-4238-9a75-26d06b1dc244">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b1372d0e-cfd1-448a-8334-bdb60fa40727" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9989,20 +9991,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1ffeec27-f743-4238-9a75-26d06b1dc244">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b1372d0e-cfd1-448a-8334-bdb60fa40727" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2696125F-A2E3-4A84-905B-AE58970A1170}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6CEBCB2-FF40-4D9B-BFCF-7AA5436CE48A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1ffeec27-f743-4238-9a75-26d06b1dc244"/>
+    <ds:schemaRef ds:uri="b1372d0e-cfd1-448a-8334-bdb60fa40727"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10027,12 +10030,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6CEBCB2-FF40-4D9B-BFCF-7AA5436CE48A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2696125F-A2E3-4A84-905B-AE58970A1170}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1ffeec27-f743-4238-9a75-26d06b1dc244"/>
-    <ds:schemaRef ds:uri="b1372d0e-cfd1-448a-8334-bdb60fa40727"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>